<commit_message>
From dev build of North Star 2.0.0
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 1.0.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3E52D73C-1258-BE42-B220-606649FAF5B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C9506D98-D42B-8743-964D-8BC0F1150CD3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Custom DCA Calculator" sheetId="1" r:id="rId1"/>
+    <sheet name="Default Settings DCA Calc" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>DCA LV</t>
   </si>
@@ -31,59 +31,10 @@
     <t>Cumulative Cost</t>
   </si>
   <si>
-    <t>Base Pair Cost =&gt;</t>
-  </si>
-  <si>
     <t>Available Balance</t>
   </si>
   <si>
-    <t>ALL_max_cost_percentage</t>
-  </si>
-  <si>
     <t># Trading Pairs</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Edit the values in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>yellow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Goal:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Total cost &lt; Available Balance</t>
-    </r>
-  </si>
-  <si>
-    <t>No DCA (Pairs Log) Qauntity</t>
   </si>
   <si>
     <t>DCA 1 Quantity</t>
@@ -103,6 +54,86 @@
   <si>
     <t>DCA Percentage</t>
   </si>
+  <si>
+    <t>DCA 5 Quantity</t>
+  </si>
+  <si>
+    <t>DCA 6 Quantity</t>
+  </si>
+  <si>
+    <t>No DCA (Pairs Log) Quantity</t>
+  </si>
+  <si>
+    <t>The North Star Settings: DCA Calculator for "Default"</t>
+  </si>
+  <si>
+    <t>DEFAULT_initial_cost_percentage</t>
+  </si>
+  <si>
+    <t>Base Pair Cost</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Value in yellow needs to be set by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>you</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+Values in Orange are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>recommendations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+Do not use negative values for DCA triggers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Goal:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Total Cost &lt; Available Balance</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -112,7 +143,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,27 +161,63 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="22"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +233,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -351,49 +436,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,123 +830,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31B4C08-E256-4B4C-8ADB-0C6869AF8304}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="26" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="8" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="8" customWidth="1"/>
+    <col min="9" max="26" width="10.6640625" style="8" customWidth="1"/>
+    <col min="27" max="16384" width="14.5" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <f>F2+(F2*C2*(1-B2))</f>
-        <v>0.10868749999999999</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="15">
-        <f>D7*D8</f>
-        <v>5.8749999999999997E-2</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <f>D2+(D2*C3*(1-B3))</f>
-        <v>0.19346374999999999</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -844,24 +901,29 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
-        <f>D3+(D3*C4*(1-B4))</f>
-        <v>0.3192151875</v>
+      <c r="B4" s="13">
+        <v>5.5E-2</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <f>F4+(F4*C4*(1-B4))</f>
+        <v>0.10034255</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="34">
+        <f>D11*D12</f>
+        <v>5.1590000000000004E-2</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -881,24 +943,24 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>2</v>
       </c>
-      <c r="B5" s="6">
-        <v>0.35</v>
+      <c r="B5" s="15">
+        <v>0.10249999999999999</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
+      <c r="C5" s="16">
+        <v>0.41</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f>D4+(D4*C5*(1-B5))</f>
-        <v>0.52670505937500001</v>
+        <v>0.13726609983624999</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -918,15 +980,24 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.41</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D9" si="0">D5+(D5*C6*(1-B6))</f>
+        <v>0.1851033356291831</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -947,18 +1018,23 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="7">
-        <v>1.25</v>
+      <c r="B7" s="13">
+        <v>0.185</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="14">
+        <v>0.41</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24695561522967463</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -979,22 +1055,23 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="9">
-        <v>4.7E-2</v>
+      <c r="B8" s="13">
+        <v>0.22</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>6</v>
+      <c r="C8" s="14">
+        <v>0.41</v>
       </c>
-      <c r="F8" s="29" t="s">
-        <v>7</v>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32593202098012458</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1015,20 +1092,23 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
-        <v>8</v>
+      <c r="A9" s="3">
+        <v>6</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="7">
-        <v>5</v>
+      <c r="B9" s="17">
+        <v>0.35</v>
       </c>
-      <c r="E9" s="27">
-        <v>10</v>
+      <c r="C9" s="18">
+        <v>1</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.53778783461720558</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1049,18 +1129,14 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="7">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1081,18 +1157,18 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>10</v>
+      <c r="A11" s="44" t="s">
+        <v>3</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="11">
-        <v>2</v>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="5">
+        <v>1.54</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1113,18 +1189,22 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>11</v>
+      <c r="A12" s="44" t="s">
+        <v>15</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="7">
-        <v>1</v>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="13">
+        <v>3.3500000000000002E-2</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
+      <c r="E12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1145,18 +1225,21 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
-        <v>12</v>
+      <c r="A13" s="44" t="s">
+        <v>13</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="11">
-        <v>0</v>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="19">
+        <v>5</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+      <c r="E13" s="53">
+        <f>SUM(D13:D19)</f>
+        <v>10</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1177,19 +1260,18 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+      <c r="A14" s="26" t="s">
+        <v>5</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="5">
-        <f>(D9*(D7*D8))+(D10*D2)+(D11*D3)+(D12*D4)+(D13*D5)</f>
-        <v>1.2172676874999999</v>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="19">
+        <v>2</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1210,14 +1292,18 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="20">
+        <v>0</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1238,17 +1324,18 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="str">
-        <f>IF(D14&gt;D7, "Over Extended! Reduce max_cost_percentage, increase balance, or lower number of pairs.", "You have enough capital for this setup")</f>
-        <v>You have enough capital for this setup</v>
+      <c r="A16" s="26" t="s">
+        <v>7</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="20">
+        <v>2</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1269,14 +1356,18 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="A17" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="21">
+        <v>0</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1297,10 +1388,18 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="54"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1321,10 +1420,18 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="21">
+        <v>0</v>
+      </c>
+      <c r="E19" s="56"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1345,10 +1452,19 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4">
+        <f>(D13*(D11*D12))+(D14*D4)+(D15*D5)+(D16*D6)+(D17*D7)+(D18*D8)+(D19*D9)</f>
+        <v>1.1547737922384909</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -1373,6 +1489,10 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1393,14 +1513,17 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="A22" s="25" t="str">
+        <f>IF(D20&gt;D11,"Over Extended! Reduce max_cost_percentage, increase balance, or lower number of pairs.",IF(D20&gt;D11*0.75,"This is more than 75% of your capital, but you have enough.","You have enough capital for this setup"))</f>
+        <v>You have enough capital for this setup</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1453,10 +1576,6 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1481,10 +1600,6 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1509,10 +1624,6 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1537,10 +1648,6 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -28692,20 +28799,190 @@
       <c r="Y996" s="2"/>
       <c r="Z996" s="2"/>
     </row>
+    <row r="997" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A997" s="2"/>
+      <c r="B997" s="2"/>
+      <c r="C997" s="2"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="2"/>
+      <c r="F997" s="2"/>
+      <c r="G997" s="2"/>
+      <c r="H997" s="2"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="2"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="2"/>
+      <c r="M997" s="2"/>
+      <c r="N997" s="2"/>
+      <c r="O997" s="2"/>
+      <c r="P997" s="2"/>
+      <c r="Q997" s="2"/>
+      <c r="R997" s="2"/>
+      <c r="S997" s="2"/>
+      <c r="T997" s="2"/>
+      <c r="U997" s="2"/>
+      <c r="V997" s="2"/>
+      <c r="W997" s="2"/>
+      <c r="X997" s="2"/>
+      <c r="Y997" s="2"/>
+      <c r="Z997" s="2"/>
+    </row>
+    <row r="998" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A998" s="2"/>
+      <c r="B998" s="2"/>
+      <c r="C998" s="2"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="2"/>
+      <c r="F998" s="2"/>
+      <c r="G998" s="2"/>
+      <c r="H998" s="2"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="2"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="2"/>
+      <c r="M998" s="2"/>
+      <c r="N998" s="2"/>
+      <c r="O998" s="2"/>
+      <c r="P998" s="2"/>
+      <c r="Q998" s="2"/>
+      <c r="R998" s="2"/>
+      <c r="S998" s="2"/>
+      <c r="T998" s="2"/>
+      <c r="U998" s="2"/>
+      <c r="V998" s="2"/>
+      <c r="W998" s="2"/>
+      <c r="X998" s="2"/>
+      <c r="Y998" s="2"/>
+      <c r="Z998" s="2"/>
+    </row>
+    <row r="999" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="2"/>
+      <c r="B999" s="2"/>
+      <c r="C999" s="2"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="2"/>
+      <c r="F999" s="2"/>
+      <c r="G999" s="2"/>
+      <c r="H999" s="2"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="2"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="2"/>
+      <c r="M999" s="2"/>
+      <c r="N999" s="2"/>
+      <c r="O999" s="2"/>
+      <c r="P999" s="2"/>
+      <c r="Q999" s="2"/>
+      <c r="R999" s="2"/>
+      <c r="S999" s="2"/>
+      <c r="T999" s="2"/>
+      <c r="U999" s="2"/>
+      <c r="V999" s="2"/>
+      <c r="W999" s="2"/>
+      <c r="X999" s="2"/>
+      <c r="Y999" s="2"/>
+      <c r="Z999" s="2"/>
+    </row>
+    <row r="1000" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1000" s="2"/>
+      <c r="B1000" s="2"/>
+      <c r="C1000" s="2"/>
+      <c r="D1000" s="2"/>
+      <c r="E1000" s="2"/>
+      <c r="F1000" s="2"/>
+      <c r="G1000" s="2"/>
+      <c r="H1000" s="2"/>
+      <c r="I1000" s="2"/>
+      <c r="J1000" s="2"/>
+      <c r="K1000" s="2"/>
+      <c r="L1000" s="2"/>
+      <c r="M1000" s="2"/>
+      <c r="N1000" s="2"/>
+      <c r="O1000" s="2"/>
+      <c r="P1000" s="2"/>
+      <c r="Q1000" s="2"/>
+      <c r="R1000" s="2"/>
+      <c r="S1000" s="2"/>
+      <c r="T1000" s="2"/>
+      <c r="U1000" s="2"/>
+      <c r="V1000" s="2"/>
+      <c r="W1000" s="2"/>
+      <c r="X1000" s="2"/>
+      <c r="Y1000" s="2"/>
+      <c r="Z1000" s="2"/>
+    </row>
+    <row r="1001" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+    </row>
+    <row r="1002" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="2"/>
+      <c r="C1002" s="2"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="2"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="2"/>
+      <c r="M1002" s="2"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+      <c r="R1002" s="2"/>
+      <c r="S1002" s="2"/>
+      <c r="T1002" s="2"/>
+      <c r="U1002" s="2"/>
+      <c r="V1002" s="2"/>
+      <c r="W1002" s="2"/>
+      <c r="X1002" s="2"/>
+      <c r="Y1002" s="2"/>
+      <c r="Z1002" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="F4:H9"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F12:H19"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:H5"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="F8:H13"/>
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Formatting and Housekeeping Update
Updated percentage formatting for cross-OS compatibility
Removed the second tab; the relevant information is in the Wiki
Removed PAIRS.properties start_balance from the bottom section
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 2.2.0 9999/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 2.3.0 A99999999/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99393035-1AC6-0B4D-B500-844091023FBC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4CB2F6DD-E64A-D041-AE58-3B4991AC9B6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Default DCA Calc" sheetId="2" r:id="rId1"/>
-    <sheet name="Example for settings.analyzer" sheetId="4" r:id="rId2"/>
+    <sheet name="DCA Calc" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>DCA LV</t>
   </si>
@@ -58,141 +57,6 @@
   <si>
     <t>Cost per Pair* 
 (Downtrend Trading)</t>
-  </si>
-  <si>
-    <t>**See next page for example of settings.analyzer.json required user settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "SettingName": "MainCurrencyTrendWarning",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "TriggerConnection": "OR",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "Triggers": [</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MarketTrendName": "MainCurrency3h",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MinChange": 4.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MarketTrendName": "MainCurrency24h",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MinChange": 5.00,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MaxChange": 8.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MaxChange": -3.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MaxChange": -4.50,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            "MinChange": -8.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        ],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "PairsProperties": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          //User Configuration Needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          "DEFAULT_sell_only_mode_enabled": false,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">          //Buy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_A_buy_strategy": "RSI",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_A_buy_value": 40.00,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_B_buy_strategy": "LOWBB",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_B_buy_value": -10.00,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_B_buy_value_limit": -35.00,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_C_buy_strategy": "STOCH",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_C_buy_value": 20.00,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "DEFAULT_trailing_buy": 0.38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "DCAProperties": {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          "DEFAULT_DCA_ignore_sell_only_mode": false,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          "DEFAULT_DCA_buy_trigger_1": -6.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      },</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">          "DEFAULT_initial_cost_percentage": </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="2"/>
-      </rPr>
-      <t>1.10,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">          "max_trading_pairs":</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 16,</t>
-    </r>
   </si>
   <si>
     <t>Validations:</t>
@@ -298,6 +162,9 @@
       <t>Does not take into consideration activiation of "Knockout Punch"</t>
     </r>
   </si>
+  <si>
+    <t>**See the configuration instructions for a picture of where to make the above changes</t>
+  </si>
 </sst>
 </file>
 
@@ -307,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -353,26 +220,6 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
@@ -828,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -929,9 +776,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -948,12 +792,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -977,9 +815,28 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -989,29 +846,26 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1019,34 +873,24 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1436,10 +1280,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA998"/>
+  <dimension ref="A1:AA997"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+      <selection activeCell="B2" sqref="B2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1461,147 +1305,147 @@
   <sheetData>
     <row r="1" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
-        <v>57</v>
+      <c r="B2" s="91" t="s">
+        <v>20</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="79" t="s">
-        <v>53</v>
+      <c r="B3" s="85" t="s">
+        <v>16</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="87"/>
     </row>
     <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="106" t="s">
-        <v>58</v>
+      <c r="B4" s="99" t="s">
+        <v>21</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="49" t="s">
-        <v>50</v>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="46" t="s">
+        <v>13</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55" t="s">
-        <v>60</v>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52" t="s">
+        <v>23</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="59">
-        <v>2.1999999999999999E-2</v>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="75">
+        <v>2.2000000000000002</v>
       </c>
-      <c r="N4" s="51"/>
+      <c r="N4" s="48"/>
       <c r="AA4" s="3">
         <f>IF(E4 = "BTC", 0.0011, 0.011)</f>
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="107" t="s">
-        <v>59</v>
+      <c r="B5" s="74" t="s">
+        <v>22</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58">
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55">
         <v>0.1</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="G5" s="47" t="s">
-        <v>61</v>
+      <c r="G5" s="44" t="s">
+        <v>24</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="60">
-        <v>1.0999999999999999E-2</v>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="76">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:27" s="33" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="79" t="s">
-        <v>49</v>
+      <c r="B6" s="85" t="s">
+        <v>12</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="87"/>
     </row>
     <row r="7" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="61" t="s">
-        <v>55</v>
+      <c r="B7" s="56" t="s">
+        <v>18</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="74" t="str">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="69" t="str">
         <f>IF(OR(E4 = "BTC", E4 = "ETH"), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>51</v>
+      <c r="B8" s="60" t="s">
+        <v>14</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="74" t="str">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="69" t="str">
         <f>IF(E4 = "BTC", IF(MIN(E12:E18) &gt;= 0.0011, "Yes", "No"), IF(MIN(E12:E18) &gt;= 0.011, "Yes", "No"))</f>
         <v>Yes</v>
       </c>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="64"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="65" t="s">
-        <v>52</v>
+      <c r="B9" s="60" t="s">
+        <v>15</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="74" t="str">
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="69" t="str">
         <f>IF(E4 = "BTC", IF(MIN(G12:G18) &gt;= 0.0011, "Yes", "No"), IF(MIN(G12:G18) &gt;= 0.011, "Yes", "No"))</f>
         <v>Yes</v>
       </c>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="67"/>
-    </row>
-    <row r="10" spans="2:27" s="104" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="105" t="s">
-        <v>63</v>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
+    </row>
+    <row r="10" spans="2:27" s="73" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="94" t="s">
+        <v>26</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="103"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="96"/>
     </row>
     <row r="11" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21" t="s">
@@ -1613,14 +1457,14 @@
       <c r="D11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="68" t="s">
-        <v>56</v>
+      <c r="E11" s="63" t="s">
+        <v>19</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="82" t="s">
+      <c r="F11" s="64"/>
+      <c r="G11" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="83"/>
+      <c r="H11" s="102"/>
       <c r="I11" s="34" t="s">
         <v>3</v>
       </c>
@@ -1652,16 +1496,16 @@
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="53">
-        <f>E5*J4</f>
+      <c r="E12" s="50">
+        <f>E5*J4*0.01</f>
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="F12" s="8">
         <f>E12*I12</f>
         <v>6.6E-3</v>
       </c>
-      <c r="G12" s="52">
-        <f>E5*J5</f>
+      <c r="G12" s="49">
+        <f>E5*J5*0.01</f>
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="H12" s="9">
@@ -1972,11 +1816,11 @@
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
       <c r="E19" s="43">
         <f>SUM(F12:F18)</f>
         <v>4.4712344407142404E-2</v>
@@ -2011,11 +1855,11 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
       <c r="E20" s="26">
         <f>E19/E5</f>
         <v>0.44712344407142401</v>
@@ -2029,11 +1873,11 @@
         <v>0.36244722768140503</v>
       </c>
       <c r="H20" s="27"/>
-      <c r="I20" s="97" t="str">
+      <c r="I20" s="80" t="str">
         <f>CONCATENATE(SUM(I12:J18)," Pairs Total")</f>
         <v>16 Pairs Total</v>
       </c>
-      <c r="J20" s="98"/>
+      <c r="J20" s="81"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2050,64 +1894,64 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="79" t="s">
-        <v>54</v>
+      <c r="B21" s="85" t="s">
+        <v>17</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="81"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="87"/>
     </row>
     <row r="22" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="70">
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="65">
         <f>E19+G19</f>
         <v>8.0957067175282907E-2</v>
       </c>
-      <c r="F22" s="62"/>
-      <c r="G22" s="71">
+      <c r="F22" s="57"/>
+      <c r="G22" s="66">
         <f>(E19+G19)/E5</f>
         <v>0.80957067175282904</v>
       </c>
       <c r="J22" s="40"/>
     </row>
     <row r="23" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="72">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="67">
         <f>E5-E22</f>
         <v>1.9042932824717099E-2</v>
       </c>
       <c r="F23" s="41"/>
-      <c r="G23" s="73">
+      <c r="G23" s="68">
         <f>1-G22</f>
         <v>0.19042932824717096</v>
       </c>
       <c r="J23" s="42"/>
     </row>
     <row r="24" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="79" t="s">
-        <v>62</v>
+      <c r="B24" s="85" t="s">
+        <v>25</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="81"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="87"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2123,19 +1967,19 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B25" s="99" t="str">
-        <f>CONCATENATE("PAIRS.properties start_balance = ", E5)</f>
-        <v>PAIRS.properties start_balance = 0.1</v>
+    <row r="25" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="82" t="str">
+        <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
+        <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.2</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="100"/>
-      <c r="J25" s="101"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="84"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2152,18 +1996,18 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="84" t="str">
-        <f>CONCATENATE("PAIRS.properties DEFAULT_initial_cost_percentage = ", J4*100)</f>
-        <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.2</v>
+      <c r="B26" s="82" t="str">
+        <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I12:I18))</f>
+        <v>PAIRS.properties max_trading_pairs = 8</v>
       </c>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="86"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="84"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2180,18 +2024,18 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="84" t="str">
-        <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I12:I18))</f>
-        <v>PAIRS.properties max_trading_pairs = 8</v>
+      <c r="B27" s="88" t="str">
+        <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
+        <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.1</v>
       </c>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="86"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="90"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2207,19 +2051,19 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="84" t="str">
-        <f>CONCATENATE("settings.analyzer.json DEFAULT_initial_cost_percentage = ", J5*100, " **")</f>
-        <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.1 **</v>
+    <row r="28" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="37" t="str">
+        <f>CONCATENATE("settings.analyzer.json max_trading_pairs = ", SUM(I12:J18), " **")</f>
+        <v>settings.analyzer.json max_trading_pairs = 16 **</v>
       </c>
-      <c r="C28" s="85"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="86"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2236,10 +2080,7 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="37" t="str">
-        <f>CONCATENATE("settings.analyzer.json max_trading_pairs = ", SUM(I12:J18), " **")</f>
-        <v>settings.analyzer.json max_trading_pairs = 16 **</v>
-      </c>
+      <c r="B29" s="37"/>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -2263,16 +2104,18 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
+    <row r="30" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="79"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2288,32 +2131,30 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
+    <row r="35" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
     </row>
     <row r="36" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
@@ -26365,39 +26206,8 @@
       <c r="W997" s="1"/>
       <c r="X997" s="1"/>
     </row>
-    <row r="998" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B27:J27"/>
+  <mergeCells count="15">
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B3:J3"/>
@@ -26406,8 +26216,13 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B27:J27"/>
   </mergeCells>
   <conditionalFormatting sqref="G22">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
@@ -26441,248 +26256,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B96319E-9CE0-4A4E-A5EA-1886CF17E57E}">
-  <dimension ref="A1:E44"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="44"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C30" s="44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C32" s="44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="44" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
The North Star 3
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 2.3.0 A99999999/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 3.0.0 B99999999/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4CB2F6DD-E64A-D041-AE58-3B4991AC9B6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A4121FD2-B4C3-8E4B-A74C-79C6FF107D5B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>DCA LV</t>
   </si>
@@ -82,9 +82,6 @@
   <si>
     <t>Cost per Pair* 
 Default Trading</t>
-  </si>
-  <si>
-    <t>Cost and Pairs Calculator for The North Star 2.2</t>
   </si>
   <si>
     <t>Market:</t>
@@ -164,6 +161,12 @@
   </si>
   <si>
     <t>**See the configuration instructions for a picture of where to make the above changes</t>
+  </si>
+  <si>
+    <t>Keep Balance Percentage</t>
+  </si>
+  <si>
+    <t>Cost and Pairs Calculator for The North Star 3.0</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -823,6 +826,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1280,7 +1294,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA997"/>
+  <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J2"/>
@@ -1305,48 +1319,48 @@
   <sheetData>
     <row r="1" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="100"/>
+    </row>
+    <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
+    </row>
+    <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="93"/>
-    </row>
-    <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="87"/>
-    </row>
-    <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="46" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="75">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="N4" s="48"/>
       <c r="AA4" s="3">
@@ -1354,64 +1368,63 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="74" t="s">
-        <v>22</v>
+    <row r="5" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="77" t="s">
+        <v>21</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55">
-        <v>0.1</v>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79">
+        <v>0.2</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="44" t="s">
-        <v>24</v>
+      <c r="F5" s="80"/>
+      <c r="G5" s="81" t="s">
+        <v>23</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="76">
-        <v>1.1000000000000001</v>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="83">
+        <v>1.35</v>
       </c>
     </row>
-    <row r="6" spans="2:27" s="33" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+    <row r="6" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="74"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="76">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" s="33" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="87"/>
-    </row>
-    <row r="7" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="56" t="s">
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="94"/>
+    </row>
+    <row r="8" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="56" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="69" t="str">
-        <f>IF(OR(E4 = "BTC", E4 = "ETH"), "Yes", "No")</f>
-        <v>Yes</v>
-      </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
-    </row>
-    <row r="8" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="60" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="57"/>
       <c r="D8" s="58"/>
       <c r="E8" s="58"/>
       <c r="F8" s="58"/>
       <c r="G8" s="69" t="str">
-        <f>IF(E4 = "BTC", IF(MIN(E12:E18) &gt;= 0.0011, "Yes", "No"), IF(MIN(E12:E18) &gt;= 0.011, "Yes", "No"))</f>
+        <f>IF(OR(E4 = "BTC", E4 = "ETH"), "Yes", "No")</f>
         <v>Yes</v>
       </c>
       <c r="H8" s="58"/>
@@ -1420,103 +1433,72 @@
     </row>
     <row r="9" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="69" t="str">
+        <f>IF(E4 = "BTC", IF(MIN(E13:E19) &gt;= 0.0011, "Yes", "No"), IF(MIN(E13:E19) &gt;= 0.011, "Yes", "No"))</f>
+        <v>Yes</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
+    </row>
+    <row r="10" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="69" t="str">
-        <f>IF(E4 = "BTC", IF(MIN(G12:G18) &gt;= 0.0011, "Yes", "No"), IF(MIN(G12:G18) &gt;= 0.011, "Yes", "No"))</f>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="69" t="str">
+        <f>IF(E4 = "BTC", IF(MIN(G13:G19) &gt;= 0.0011, "Yes", "No"), IF(MIN(G13:G19) &gt;= 0.011, "Yes", "No"))</f>
         <v>Yes</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
-    </row>
-    <row r="10" spans="2:27" s="73" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="94" t="s">
-        <v>26</v>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
+    </row>
+    <row r="11" spans="2:27" s="73" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="101" t="s">
+        <v>25</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="96"/>
-    </row>
-    <row r="11" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="103"/>
+    </row>
+    <row r="12" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E12" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="101" t="s">
+      <c r="F12" s="64"/>
+      <c r="G12" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="102"/>
-      <c r="I11" s="34" t="s">
+      <c r="H12" s="109"/>
+      <c r="I12" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J12" s="22" t="s">
         <v>4</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-    </row>
-    <row r="12" spans="2:27" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="50">
-        <f>E5*J4*0.01</f>
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="F12" s="8">
-        <f>E12*I12</f>
-        <v>6.6E-3</v>
-      </c>
-      <c r="G12" s="49">
-        <f>E5*J5*0.01</f>
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="H12" s="9">
-        <f>G12*J12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="35">
-        <v>3</v>
-      </c>
-      <c r="J12" s="30">
-        <v>0</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1533,84 +1515,84 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="24">
+    <row r="13" spans="2:27" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="50">
+        <f>E5*J6*J4*0.0001</f>
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="F13" s="8">
+        <f>E13*I13</f>
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="G13" s="49">
+        <f>E5*J6*J5*0.0001</f>
+        <v>1.3500000000000001E-3</v>
+      </c>
+      <c r="H13" s="9">
+        <f>G13*J13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="35">
+        <v>3</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+    </row>
+    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="24">
         <v>1</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="12">
         <v>6.1699999999999998E-2</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="10">
-        <f t="shared" ref="E13:E18" si="0">E12+(E12*D13*(1-C13))</f>
-        <v>4.2642600000000006E-3</v>
+      <c r="E14" s="10">
+        <f t="shared" ref="E14:E19" si="0">E13+(E13*D14*(1-C14))</f>
+        <v>5.2334100000000008E-3</v>
       </c>
-      <c r="F13" s="8">
-        <f t="shared" ref="F13:F18" si="1">E13*I13</f>
-        <v>8.5285200000000012E-3</v>
+      <c r="F14" s="8">
+        <f t="shared" ref="F14:F19" si="1">E14*I14</f>
+        <v>1.0466820000000002E-2</v>
       </c>
-      <c r="G13" s="10">
-        <f t="shared" ref="G13:G18" si="2">G12+(G12*D13*(1-C13))</f>
-        <v>2.1321300000000003E-3</v>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:G19" si="2">G13+(G13*D14*(1-C14))</f>
+        <v>2.6167050000000004E-3</v>
       </c>
-      <c r="H13" s="9">
-        <f t="shared" ref="H13:H18" si="3">G13*J13</f>
-        <v>2.1321300000000003E-3</v>
+      <c r="H14" s="9">
+        <f t="shared" ref="H14:H19" si="3">G14*J14</f>
+        <v>2.6167050000000004E-3</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I14" s="35">
         <v>2</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J14" s="30">
         <v>1</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-    </row>
-    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="24">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.41</v>
-      </c>
-      <c r="E14" s="10">
-        <f t="shared" si="0"/>
-        <v>5.8334010735000006E-3</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="10">
-        <f t="shared" si="2"/>
-        <v>2.9167005367500003E-3</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="3"/>
-        <v>5.8334010735000006E-3</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0</v>
-      </c>
-      <c r="J14" s="30">
-        <v>2</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1629,35 +1611,35 @@
     </row>
     <row r="15" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="12">
-        <v>0.15</v>
+        <v>0.10249999999999999</v>
       </c>
       <c r="D15" s="13">
         <v>0.41</v>
       </c>
       <c r="E15" s="10">
         <f t="shared" si="0"/>
-        <v>7.8663413476147501E-3</v>
+        <v>7.1591740447500014E-3</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="1"/>
-        <v>1.57326826952295E-2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="10">
         <f t="shared" si="2"/>
-        <v>3.9331706738073751E-3</v>
+        <v>3.5795870223750007E-3</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="3"/>
-        <v>3.9331706738073751E-3</v>
+        <v>7.1591740447500014E-3</v>
       </c>
       <c r="I15" s="35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1674,37 +1656,37 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="12">
-        <v>0.185</v>
+        <v>0.15</v>
       </c>
       <c r="D16" s="13">
         <v>0.41</v>
       </c>
       <c r="E16" s="10">
         <f t="shared" si="0"/>
-        <v>1.0494879308920218E-2</v>
+        <v>9.6541461993453759E-3</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9308292398690752E-2</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" si="2"/>
-        <v>5.2474396544601089E-3</v>
+        <v>4.8270730996726879E-3</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="3"/>
-        <v>1.0494879308920218E-2</v>
+        <v>4.8270730996726879E-3</v>
       </c>
       <c r="I16" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1723,32 +1705,32 @@
     </row>
     <row r="17" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="12">
-        <v>0.22</v>
+        <v>0.185</v>
       </c>
       <c r="D17" s="13">
         <v>0.41</v>
       </c>
       <c r="E17" s="10">
         <f t="shared" si="0"/>
-        <v>1.3851141711912904E-2</v>
+        <v>1.2880079151856634E-2</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="1"/>
-        <v>1.3851141711912904E-2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" si="2"/>
-        <v>6.9255708559564522E-3</v>
+        <v>6.440039575928317E-3</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="3"/>
-        <v>1.3851141711912904E-2</v>
+        <v>1.2880079151856634E-2</v>
       </c>
       <c r="I17" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="30">
         <v>2</v>
@@ -1768,37 +1750,37 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
-        <v>6</v>
+    <row r="18" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="24">
+        <v>5</v>
       </c>
-      <c r="C18" s="14">
-        <v>0.35</v>
+      <c r="C18" s="12">
+        <v>0.22</v>
       </c>
-      <c r="D18" s="15">
-        <v>1</v>
+      <c r="D18" s="13">
+        <v>0.41</v>
       </c>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>2.2854383824656294E-2</v>
+        <v>1.6999128464620386E-2</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6999128464620386E-2</v>
       </c>
       <c r="G18" s="10">
         <f t="shared" si="2"/>
-        <v>1.1427191912328147E-2</v>
+        <v>8.499564232310193E-3</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.6999128464620386E-2</v>
       </c>
-      <c r="I18" s="36">
-        <v>0</v>
+      <c r="I18" s="35">
+        <v>1</v>
       </c>
-      <c r="J18" s="31">
-        <v>0</v>
+      <c r="J18" s="30">
+        <v>2</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1815,29 +1797,37 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="97" t="s">
-        <v>7</v>
+    <row r="19" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25">
+        <v>6</v>
       </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="43">
-        <f>SUM(F12:F18)</f>
-        <v>4.4712344407142404E-2</v>
+      <c r="C19" s="14">
+        <v>0.35</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19">
-        <f>SUM(H12:H18)</f>
-        <v>3.6244722768140503E-2</v>
+      <c r="D19" s="15">
+        <v>1</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="29" t="str">
-        <f>CONCATENATE(SUM(I12:I18), " Pairs")</f>
-        <v>8 Pairs</v>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8048561966623635E-2</v>
       </c>
-      <c r="J19" s="32" t="str">
-        <f>CONCATENATE(SUM(J12:J18), " Pairs")</f>
-        <v>8 Pairs</v>
+      <c r="F19" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="2"/>
+        <v>1.4024280983311817E-2</v>
+      </c>
+      <c r="H19" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="36">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31">
+        <v>0</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1854,30 +1844,30 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="103" t="s">
-        <v>10</v>
+    <row r="20" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="104" t="s">
+        <v>7</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="26">
-        <f>E19/E5</f>
-        <v>0.44712344407142401</v>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="43">
+        <f>SUM(F13:F19)</f>
+        <v>5.4874240863311136E-2</v>
       </c>
-      <c r="F20" s="26" t="e">
-        <f>F19/C4</f>
-        <v>#DIV/0!</v>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19">
+        <f>SUM(H13:H19)</f>
+        <v>4.4482159760899712E-2</v>
       </c>
-      <c r="G20" s="26">
-        <f>G19/E5</f>
-        <v>0.36244722768140503</v>
+      <c r="H20" s="20"/>
+      <c r="I20" s="29" t="str">
+        <f>CONCATENATE(SUM(I13:I19), " Pairs")</f>
+        <v>8 Pairs</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="80" t="str">
-        <f>CONCATENATE(SUM(I12:J18)," Pairs Total")</f>
-        <v>16 Pairs Total</v>
+      <c r="J20" s="32" t="str">
+        <f>CONCATENATE(SUM(J13:J19), " Pairs")</f>
+        <v>8 Pairs</v>
       </c>
-      <c r="J20" s="81"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1893,93 +1883,104 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="85" t="s">
+    <row r="21" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="110" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="26">
+        <f>E20/E5</f>
+        <v>0.27437120431655565</v>
+      </c>
+      <c r="F21" s="26" t="e">
+        <f>F20/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="26">
+        <f>G20/E5</f>
+        <v>0.22241079880449854</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="87" t="str">
+        <f>CONCATENATE(SUM(I13:J19)," Pairs Total")</f>
+        <v>16 Pairs Total</v>
+      </c>
+      <c r="J21" s="88"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="87"/>
-    </row>
-    <row r="22" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="70" t="s">
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="94"/>
+    </row>
+    <row r="23" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="65">
-        <f>E19+G19</f>
-        <v>8.0957067175282907E-2</v>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="65">
+        <f>E20+G20</f>
+        <v>9.9356400624210847E-2</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="66">
-        <f>(E19+G19)/E5</f>
-        <v>0.80957067175282904</v>
+      <c r="F23" s="57"/>
+      <c r="G23" s="66">
+        <f>(E20+G20)/E5</f>
+        <v>0.49678200312105419</v>
       </c>
-      <c r="J22" s="40"/>
-    </row>
-    <row r="23" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="72" t="s">
+      <c r="J23" s="40"/>
+    </row>
+    <row r="24" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="67">
-        <f>E5-E22</f>
-        <v>1.9042932824717099E-2</v>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="67">
+        <f>E5-E23</f>
+        <v>0.10064359937578916</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="68">
-        <f>1-G22</f>
-        <v>0.19042932824717096</v>
+      <c r="F24" s="41"/>
+      <c r="G24" s="68">
+        <f>1-G23</f>
+        <v>0.50321799687894586</v>
       </c>
-      <c r="J23" s="42"/>
-    </row>
-    <row r="24" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="85" t="s">
-        <v>25</v>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="92" t="s">
+        <v>24</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="82" t="str">
-        <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
-        <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.2</v>
-      </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="84"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="94"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1996,18 +1997,18 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="82" t="str">
-        <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I12:I18))</f>
-        <v>PAIRS.properties max_trading_pairs = 8</v>
+      <c r="B26" s="89" t="str">
+        <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
+        <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.7</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="84"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="91"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2024,18 +2025,18 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="88" t="str">
-        <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
-        <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.1</v>
+      <c r="B27" s="89" t="str">
+        <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I13:I19))</f>
+        <v>PAIRS.properties max_trading_pairs = 8</v>
       </c>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="91"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2051,19 +2052,19 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="37" t="str">
-        <f>CONCATENATE("settings.analyzer.json max_trading_pairs = ", SUM(I12:J18), " **")</f>
-        <v>settings.analyzer.json max_trading_pairs = 16 **</v>
+    <row r="28" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="95" t="str">
+        <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
+        <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.35</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="97"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2080,7 +2081,10 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
+      <c r="B29" s="37" t="str">
+        <f>CONCATENATE("settings.analyzer.json max_trading_pairs = ", SUM(I13:J19), " **")</f>
+        <v>settings.analyzer.json max_trading_pairs = 16 **</v>
+      </c>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -2104,18 +2108,16 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="79"/>
+    <row r="30" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2131,30 +2133,32 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="35" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
+    <row r="31" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
     </row>
     <row r="36" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
@@ -26206,25 +26210,50 @@
       <c r="W997" s="1"/>
       <c r="X997" s="1"/>
     </row>
+    <row r="998" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="1"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="1"/>
+      <c r="G998" s="1"/>
+      <c r="H998" s="1"/>
+      <c r="I998" s="1"/>
+      <c r="J998" s="1"/>
+      <c r="K998" s="1"/>
+      <c r="L998" s="1"/>
+      <c r="M998" s="1"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B11:J11"/>
     <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:J22"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B26:J26"/>
     <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B26:J26"/>
     <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
   </mergeCells>
-  <conditionalFormatting sqref="G22">
+  <conditionalFormatting sqref="G23">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -26232,7 +26261,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G9">
+  <conditionalFormatting sqref="G8:G10">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -26240,7 +26269,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
       <formula>$E$5</formula>
     </cfRule>
@@ -26248,7 +26277,7 @@
       <formula>$E$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:G18">
+  <conditionalFormatting sqref="E13:G19">
     <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThan">
       <formula>$AA$4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed keep_balance and initial cost equation error
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 3.0.0 B99999999/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 3.0.0 GM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A4121FD2-B4C3-8E4B-A74C-79C6FF107D5B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{79914B2B-72E3-744A-A18F-23D2BF97679A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,9 +776,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -839,30 +836,9 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -880,6 +856,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -905,6 +890,21 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,162 +1319,162 @@
   <sheetData>
     <row r="1" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="94"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="92"/>
     </row>
     <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="46" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52" t="s">
+      <c r="F4" s="50"/>
+      <c r="G4" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="75">
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="74">
         <v>2.7</v>
       </c>
-      <c r="N4" s="48"/>
+      <c r="N4" s="47"/>
       <c r="AA4" s="3">
         <f>IF(E4 = "BTC", 0.0011, 0.011)</f>
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="79">
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="78">
         <v>0.2</v>
       </c>
-      <c r="F5" s="80"/>
-      <c r="G5" s="81" t="s">
+      <c r="F5" s="79"/>
+      <c r="G5" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83">
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82">
         <v>1.35</v>
       </c>
     </row>
     <row r="6" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="74"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="28"/>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="76">
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="75">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:27" s="33" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="92"/>
     </row>
     <row r="8" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="69" t="str">
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="68" t="str">
         <f>IF(OR(E4 = "BTC", E4 = "ETH"), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="69" t="str">
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="68" t="str">
         <f>IF(E4 = "BTC", IF(MIN(E13:E19) &gt;= 0.0011, "Yes", "No"), IF(MIN(E13:E19) &gt;= 0.011, "Yes", "No"))</f>
         <v>Yes</v>
       </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="69" t="str">
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="68" t="str">
         <f>IF(E4 = "BTC", IF(MIN(G13:G19) &gt;= 0.0011, "Yes", "No"), IF(MIN(G13:G19) &gt;= 0.011, "Yes", "No"))</f>
         <v>Yes</v>
       </c>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
-    </row>
-    <row r="11" spans="2:27" s="73" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
+    </row>
+    <row r="11" spans="2:27" s="72" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="103"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="89"/>
     </row>
     <row r="12" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21" t="s">
@@ -1486,14 +1486,14 @@
       <c r="D12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="108" t="s">
+      <c r="F12" s="63"/>
+      <c r="G12" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="109"/>
+      <c r="H12" s="98"/>
       <c r="I12" s="34" t="s">
         <v>3</v>
       </c>
@@ -1525,16 +1525,16 @@
       <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="50">
-        <f>E5*J6*J4*0.0001</f>
+      <c r="E13" s="49">
+        <f>E5*(100-J6)*J4*0.0001</f>
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="F13" s="8">
         <f>E13*I13</f>
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="G13" s="49">
-        <f>E5*J6*J5*0.0001</f>
+      <c r="G13" s="48">
+        <f>E5*(100-J6)*J5*0.0001</f>
         <v>1.3500000000000001E-3</v>
       </c>
       <c r="H13" s="9">
@@ -1617,11 +1617,11 @@
         <v>0.10249999999999999</v>
       </c>
       <c r="D15" s="13">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="E15" s="10">
         <f t="shared" si="0"/>
-        <v>7.1591740447500014E-3</v>
+        <v>6.7834152067500009E-3</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="1"/>
@@ -1629,11 +1629,11 @@
       </c>
       <c r="G15" s="10">
         <f t="shared" si="2"/>
-        <v>3.5795870223750007E-3</v>
+        <v>3.3917076033750005E-3</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="3"/>
-        <v>7.1591740447500014E-3</v>
+        <v>6.7834152067500009E-3</v>
       </c>
       <c r="I15" s="35">
         <v>0</v>
@@ -1664,23 +1664,23 @@
         <v>0.15</v>
       </c>
       <c r="D16" s="13">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="E16" s="10">
         <f t="shared" si="0"/>
-        <v>9.6541461993453759E-3</v>
+        <v>9.666366669618752E-3</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="1"/>
-        <v>1.9308292398690752E-2</v>
+        <v>1.9332733339237504E-2</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" si="2"/>
-        <v>4.8270730996726879E-3</v>
+        <v>4.833183334809376E-3</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="3"/>
-        <v>4.8270730996726879E-3</v>
+        <v>4.833183334809376E-3</v>
       </c>
       <c r="I16" s="35">
         <v>2</v>
@@ -1711,11 +1711,11 @@
         <v>0.185</v>
       </c>
       <c r="D17" s="13">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="E17" s="10">
         <f t="shared" si="0"/>
-        <v>1.2880079151856634E-2</v>
+        <v>1.2266135985412716E-2</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="1"/>
@@ -1723,11 +1723,11 @@
       </c>
       <c r="G17" s="10">
         <f t="shared" si="2"/>
-        <v>6.440039575928317E-3</v>
+        <v>6.1330679927063579E-3</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="3"/>
-        <v>1.2880079151856634E-2</v>
+        <v>1.2266135985412716E-2</v>
       </c>
       <c r="I17" s="35">
         <v>0</v>
@@ -1758,23 +1758,23 @@
         <v>0.22</v>
       </c>
       <c r="D18" s="13">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>1.6999128464620386E-2</v>
+        <v>1.7049929019723676E-2</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>1.6999128464620386E-2</v>
+        <v>1.7049929019723676E-2</v>
       </c>
       <c r="G18" s="10">
         <f t="shared" si="2"/>
-        <v>8.499564232310193E-3</v>
+        <v>8.524964509861838E-3</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="3"/>
-        <v>1.6999128464620386E-2</v>
+        <v>1.7049929019723676E-2</v>
       </c>
       <c r="I18" s="35">
         <v>1</v>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="E19" s="10">
         <f t="shared" si="0"/>
-        <v>2.8048561966623635E-2</v>
+        <v>2.8132382882544067E-2</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="1"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="G19" s="10">
         <f t="shared" si="2"/>
-        <v>1.4024280983311817E-2</v>
+        <v>1.4066191441272033E-2</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" si="3"/>
@@ -1845,19 +1845,19 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="43">
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="83">
         <f>SUM(F13:F19)</f>
-        <v>5.4874240863311136E-2</v>
+        <v>5.4949482358961174E-2</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="19">
         <f>SUM(H13:H19)</f>
-        <v>4.4482159760899712E-2</v>
+        <v>4.3549368546695763E-2</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="29" t="str">
@@ -1884,14 +1884,14 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
       <c r="E21" s="26">
         <f>E20/E5</f>
-        <v>0.27437120431655565</v>
+        <v>0.27474741179480583</v>
       </c>
       <c r="F21" s="26" t="e">
         <f>F20/C4</f>
@@ -1899,14 +1899,14 @@
       </c>
       <c r="G21" s="26">
         <f>G20/E5</f>
-        <v>0.22241079880449854</v>
+        <v>0.2177468427334788</v>
       </c>
       <c r="H21" s="27"/>
-      <c r="I21" s="87" t="str">
+      <c r="I21" s="104" t="str">
         <f>CONCATENATE(SUM(I13:J19)," Pairs Total")</f>
         <v>16 Pairs Total</v>
       </c>
-      <c r="J21" s="88"/>
+      <c r="J21" s="105"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1923,64 +1923,64 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="93"/>
-      <c r="J22" s="94"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="92"/>
     </row>
     <row r="23" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="65">
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="64">
         <f>E20+G20</f>
-        <v>9.9356400624210847E-2</v>
+        <v>9.8498850905656937E-2</v>
       </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="66">
+      <c r="F23" s="56"/>
+      <c r="G23" s="65">
         <f>(E20+G20)/E5</f>
-        <v>0.49678200312105419</v>
+        <v>0.49249425452828466</v>
       </c>
       <c r="J23" s="40"/>
     </row>
     <row r="24" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="67">
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="66">
         <f>E5-E23</f>
-        <v>0.10064359937578916</v>
+        <v>0.10150114909434307</v>
       </c>
       <c r="F24" s="41"/>
-      <c r="G24" s="68">
+      <c r="G24" s="67">
         <f>1-G23</f>
-        <v>0.50321799687894586</v>
+        <v>0.50750574547171534</v>
       </c>
       <c r="J24" s="42"/>
     </row>
     <row r="25" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="94"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="91"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="92"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1997,18 +1997,18 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="89" t="str">
+      <c r="B26" s="106" t="str">
         <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
         <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.7</v>
       </c>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="91"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="108"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2025,18 +2025,18 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="89" t="str">
+      <c r="B27" s="106" t="str">
         <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I13:I19))</f>
         <v>PAIRS.properties max_trading_pairs = 8</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="91"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="108"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2053,18 +2053,18 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="95" t="str">
+      <c r="B28" s="109" t="str">
         <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
         <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.35</v>
       </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="97"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="111"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2134,17 +2134,17 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="86"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="103"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -26237,6 +26237,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B3:J3"/>
@@ -26246,12 +26252,6 @@
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <conditionalFormatting sqref="G23">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">

</xml_diff>

<commit_message>
Updated cell highlighting (green vs red)
Highlighting green vs red takes into consideration keep_balance_percentage
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 3.0.0 GM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{79914B2B-72E3-744A-A18F-23D2BF97679A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{796A90AD-766D-314E-B427-B7AD9B2E6433}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -839,6 +839,30 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -856,15 +880,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,27 +905,502 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1319,37 +1809,37 @@
   <sheetData>
     <row r="1" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="86"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="94"/>
     </row>
     <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="45" t="s">
         <v>13</v>
       </c>
@@ -1403,17 +1893,17 @@
       </c>
     </row>
     <row r="7" spans="2:27" s="33" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="92"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="94"/>
     </row>
     <row r="8" spans="2:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="55" t="s">
@@ -1464,17 +1954,17 @@
       <c r="J10" s="61"/>
     </row>
     <row r="11" spans="2:27" s="72" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="103"/>
     </row>
     <row r="12" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21" t="s">
@@ -1490,10 +1980,10 @@
         <v>19</v>
       </c>
       <c r="F12" s="63"/>
-      <c r="G12" s="97" t="s">
+      <c r="G12" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="98"/>
+      <c r="H12" s="109"/>
       <c r="I12" s="34" t="s">
         <v>3</v>
       </c>
@@ -1845,11 +2335,11 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
       <c r="E20" s="83">
         <f>SUM(F13:F19)</f>
         <v>5.4949482358961174E-2</v>
@@ -1884,11 +2374,11 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
       <c r="E21" s="26">
         <f>E20/E5</f>
         <v>0.27474741179480583</v>
@@ -1902,11 +2392,11 @@
         <v>0.2177468427334788</v>
       </c>
       <c r="H21" s="27"/>
-      <c r="I21" s="104" t="str">
+      <c r="I21" s="87" t="str">
         <f>CONCATENATE(SUM(I13:J19)," Pairs Total")</f>
         <v>16 Pairs Total</v>
       </c>
-      <c r="J21" s="105"/>
+      <c r="J21" s="88"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1923,17 +2413,17 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="90" t="s">
+      <c r="B22" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="92"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="94"/>
     </row>
     <row r="23" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="69" t="s">
@@ -1970,17 +2460,17 @@
       <c r="J24" s="42"/>
     </row>
     <row r="25" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="92"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="94"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1997,18 +2487,18 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="106" t="str">
+      <c r="B26" s="89" t="str">
         <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
         <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.7</v>
       </c>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="108"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="91"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2025,18 +2515,18 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="106" t="str">
+      <c r="B27" s="89" t="str">
         <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I13:I19))</f>
         <v>PAIRS.properties max_trading_pairs = 8</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="108"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="91"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2053,18 +2543,18 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="109" t="str">
+      <c r="B28" s="95" t="str">
         <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
         <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.35</v>
       </c>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="111"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="97"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2134,17 +2624,17 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="102"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="103"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="86"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -26237,12 +26727,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B3:J3"/>
@@ -26252,33 +26736,39 @@
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <conditionalFormatting sqref="G23">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThanOrEqual">
+      <formula>$J$6*0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
+      <formula>$J$6*0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G10">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
-      <formula>$E$5</formula>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThanOrEqual">
+      <formula>$E$5*0.01*(100-$J$6)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
-      <formula>$E$5</formula>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+      <formula>$E$5*0.01*(100-$J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:G19">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
       <formula>$AA$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Improvements for clarity - we're listening to you!
</commit_message>
<xml_diff>
--- a/pairs_setup.xlsx
+++ b/pairs_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Crypto/The North Star 3.0.0 GM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{796A90AD-766D-314E-B427-B7AD9B2E6433}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{858EBCAA-60EA-064A-9932-71DB642C58F7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>DCA LV</t>
   </si>
@@ -168,6 +168,18 @@
   <si>
     <t>Cost and Pairs Calculator for The North Star 3.0</t>
   </si>
+  <si>
+    <t>Lower Risk Profile</t>
+  </si>
+  <si>
+    <t>Higher Risk Profile</t>
+  </si>
+  <si>
+    <t>(Default Global, Uptrend, PAIRS, etc.)</t>
+  </si>
+  <si>
+    <t>(Downtrend, Warning, Critical, etc.)</t>
+  </si>
 </sst>
 </file>
 
@@ -256,7 +268,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +320,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,7 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -839,30 +863,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -880,6 +882,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -905,502 +916,53 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1786,8 +1348,8 @@
   </sheetPr>
   <dimension ref="A1:AA998"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1809,17 +1371,17 @@
   <sheetData>
     <row r="1" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="2:27" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="92" t="s">
@@ -1835,11 +1397,11 @@
       <c r="J3" s="94"/>
     </row>
     <row r="4" spans="2:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="45" t="s">
         <v>13</v>
       </c>
@@ -1954,17 +1516,17 @@
       <c r="J10" s="61"/>
     </row>
     <row r="11" spans="2:27" s="72" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="103"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="91"/>
     </row>
     <row r="12" spans="2:27" s="6" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21" t="s">
@@ -1980,10 +1542,10 @@
         <v>19</v>
       </c>
       <c r="F12" s="63"/>
-      <c r="G12" s="108" t="s">
+      <c r="G12" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="109"/>
+      <c r="H12" s="100"/>
       <c r="I12" s="34" t="s">
         <v>3</v>
       </c>
@@ -2335,11 +1897,11 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" s="3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
       <c r="E20" s="83">
         <f>SUM(F13:F19)</f>
         <v>5.4949482358961174E-2</v>
@@ -2374,11 +1936,11 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="26">
         <f>E20/E5</f>
         <v>0.27474741179480583</v>
@@ -2392,11 +1954,11 @@
         <v>0.2177468427334788</v>
       </c>
       <c r="H21" s="27"/>
-      <c r="I21" s="87" t="str">
+      <c r="I21" s="106" t="str">
         <f>CONCATENATE(SUM(I13:J19)," Pairs Total")</f>
         <v>16 Pairs Total</v>
       </c>
-      <c r="J21" s="88"/>
+      <c r="J21" s="107"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2487,18 +2049,20 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="89" t="str">
-        <f>"PAIRS.properties DEFAULT_initial_cost_percentage = " &amp; J4</f>
-        <v>PAIRS.properties DEFAULT_initial_cost_percentage = 2.7</v>
+      <c r="B26" s="112" t="s">
+        <v>29</v>
       </c>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="91"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="116" t="str">
+        <f>"DEFAULT_initial_cost_percentage = " &amp; J4</f>
+        <v>DEFAULT_initial_cost_percentage = 2.7</v>
+      </c>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="108"/>
+      <c r="J26" s="109"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2515,18 +2079,20 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="89" t="str">
-        <f>CONCATENATE("PAIRS.properties max_trading_pairs = ", SUM(I13:I19))</f>
-        <v>PAIRS.properties max_trading_pairs = 8</v>
+      <c r="B27" s="118" t="s">
+        <v>31</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="91"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120" t="str">
+        <f>CONCATENATE("max_trading_pairs = ", SUM(I13:I19))</f>
+        <v>max_trading_pairs = 8</v>
+      </c>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="109"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2543,18 +2109,20 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="95" t="str">
-        <f>"settings.analyzer.json DEFAULT_initial_cost_percentage = " &amp; J5</f>
-        <v>settings.analyzer.json DEFAULT_initial_cost_percentage = 1.35</v>
+      <c r="B28" s="114" t="s">
+        <v>30</v>
       </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="97"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="117" t="str">
+        <f>"DEFAULT_initial_cost_percentage = " &amp; J5</f>
+        <v>DEFAULT_initial_cost_percentage = 1.35</v>
+      </c>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="111"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2571,18 +2139,20 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="2:24" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="37" t="str">
-        <f>CONCATENATE("settings.analyzer.json max_trading_pairs = ", SUM(I13:J19), " **")</f>
-        <v>settings.analyzer.json max_trading_pairs = 16 **</v>
+      <c r="B29" s="121" t="s">
+        <v>32</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="122"/>
+      <c r="E29" s="123" t="str">
+        <f>CONCATENATE("max_trading_pairs = ", SUM(I13:J19), " **")</f>
+        <v>max_trading_pairs = 16 **</v>
+      </c>
+      <c r="F29" s="123"/>
+      <c r="G29" s="123"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="85"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2624,17 +2194,17 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="86"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="105"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -26726,7 +26296,14 @@
       <c r="X998" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B3:J3"/>
@@ -26736,39 +26313,33 @@
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <conditionalFormatting sqref="G23">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThanOrEqual">
       <formula>$J$6*0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>$J$6*0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G10">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThanOrEqual">
       <formula>$E$5*0.01*(100-$J$6)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
       <formula>$E$5*0.01*(100-$J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:G19">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThan">
       <formula>$AA$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>